<commit_message>
update channel reaches 3/10/21
</commit_message>
<xml_diff>
--- a/issue_checklists/NCF_LMR.xlsx
+++ b/issue_checklists/NCF_LMR.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrews\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrews\NCF\issue_checklists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9746A5B9-F32E-40FA-B7DC-D5AB2941BF9E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C794BDF1-BE77-4AA3-B4DA-6737A68D4B69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{4188A33A-E0A9-4B65-A79B-6B8CE0ECD579}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{4188A33A-E0A9-4B65-A79B-6B8CE0ECD579}"/>
   </bookViews>
   <sheets>
     <sheet name="RMs" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8455" uniqueCount="2589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8461" uniqueCount="2590">
   <si>
     <t>FID</t>
   </si>
@@ -7804,6 +7804,9 @@
   </si>
   <si>
     <t>remove CLD reaches, keep OVL reaches</t>
+  </si>
+  <si>
+    <t>combined into a single reach</t>
   </si>
 </sst>
 </file>
@@ -8287,7 +8290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2964B595-0063-4E70-978A-D728233CC9C0}">
   <dimension ref="A1:AC814"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AG23" sqref="AG23"/>
     </sheetView>
   </sheetViews>
@@ -51726,8 +51729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD898DBE-B658-4D5F-9524-2DBDF77B69A9}">
   <dimension ref="A1:I136"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H132" sqref="H132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53977,8 +53980,12 @@
       <c r="D131" s="4" t="s">
         <v>1631</v>
       </c>
-      <c r="E131" s="4"/>
-      <c r="F131" s="4"/>
+      <c r="E131" s="4" t="s">
+        <v>2585</v>
+      </c>
+      <c r="F131" s="4" t="s">
+        <v>2589</v>
+      </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
@@ -53993,8 +54000,12 @@
       <c r="D132" s="4" t="s">
         <v>1627</v>
       </c>
-      <c r="E132" s="4"/>
-      <c r="F132" s="4"/>
+      <c r="E132" s="4" t="s">
+        <v>2585</v>
+      </c>
+      <c r="F132" s="4" t="s">
+        <v>2589</v>
+      </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
@@ -54009,8 +54020,12 @@
       <c r="D133" s="4" t="s">
         <v>1623</v>
       </c>
-      <c r="E133" s="4"/>
-      <c r="F133" s="4"/>
+      <c r="E133" s="4" t="s">
+        <v>2585</v>
+      </c>
+      <c r="F133" s="4" t="s">
+        <v>2589</v>
+      </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">

</xml_diff>